<commit_message>
Added Standard Deviation to SourceMeter results
</commit_message>
<xml_diff>
--- a/results/SourceMeter/C - SourceMeter (LICCA).xlsx
+++ b/results/SourceMeter/C - SourceMeter (LICCA).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="62">
   <si>
     <t>Name </t>
   </si>
@@ -202,6 +202,15 @@
   <si>
     <t xml:space="preserve"> Licca_C:S3b.c</t>
   </si>
+  <si>
+    <t>(manually)</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>STDEV.P</t>
+  </si>
 </sst>
 </file>
 
@@ -366,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,8 +426,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,17 +720,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AM62"/>
+  <dimension ref="A2:AM64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.88671875" customWidth="1"/>
     <col min="6" max="6" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.88671875" bestFit="1" customWidth="1"/>
@@ -719,7 +740,7 @@
     <col min="10" max="10" width="5.33203125" customWidth="1"/>
     <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.6640625" bestFit="1" customWidth="1"/>
@@ -5150,6 +5171,12 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="K41" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="L41" s="30"/>
+    </row>
     <row r="42" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="10"/>
       <c r="C42" s="1" t="s">
@@ -5176,6 +5203,12 @@
       <c r="J42" s="19" t="s">
         <v>36</v>
       </c>
+      <c r="K42" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="L42" s="29" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
@@ -5213,6 +5246,14 @@
         <f>AVERAGEIF($B$3:$B$38, B43, $AL$3:$AL$38)</f>
         <v>5.5</v>
       </c>
+      <c r="K43">
+        <f>C43*LOG(D43,2)</f>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L43">
+        <f>MAX(0,(171 - 5.2 * LN(K43) - 0.23 * (E43) - 16.2 *LN(H43))*100 / 171)</f>
+        <v>69.867328586742232</v>
+      </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
@@ -5250,6 +5291,14 @@
         <f t="shared" ref="J44:J60" si="7">AVERAGEIF($B$3:$B$38, B44, $AL$3:$AL$38)</f>
         <v>5.5</v>
       </c>
+      <c r="K44">
+        <f t="shared" ref="K44:K60" si="8">C44*LOG(D44,2)</f>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ref="L44:L60" si="9">MAX(0,(171 - 5.2 * LN(K44) - 0.23 * (E44) - 16.2 *LN(H44))*100 / 171)</f>
+        <v>69.867328586742232</v>
+      </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
@@ -5287,6 +5336,14 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K45">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
@@ -5324,6 +5381,14 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="K46">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="9"/>
+        <v>69.04301027841943</v>
+      </c>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
@@ -5361,6 +5426,14 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K47">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
@@ -5398,8 +5471,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -5435,8 +5516,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K49">
+        <f t="shared" si="8"/>
+        <v>89.850829879453826</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="9"/>
+        <v>69.969413151185478</v>
+      </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -5472,8 +5561,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K50">
+        <f t="shared" si="8"/>
+        <v>105.46253196702112</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="9"/>
+        <v>69.482240376722075</v>
+      </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>47</v>
       </c>
@@ -5509,8 +5606,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K51">
+        <f t="shared" si="8"/>
+        <v>101.38196255841365</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="9"/>
+        <v>69.602237374857296</v>
+      </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>58</v>
       </c>
@@ -5546,8 +5651,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K52">
+        <f t="shared" si="8"/>
+        <v>86.03910001730776</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="9"/>
+        <v>70.101234687370663</v>
+      </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>48</v>
       </c>
@@ -5583,8 +5696,16 @@
         <f t="shared" si="7"/>
         <v>6.5</v>
       </c>
+      <c r="K53">
+        <f t="shared" si="8"/>
+        <v>113.29982727264704</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="9"/>
+        <v>67.614391220989859</v>
+      </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>49</v>
       </c>
@@ -5620,8 +5741,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K54">
+        <f t="shared" si="8"/>
+        <v>80.661656266226018</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="9"/>
+        <v>70.297492178549263</v>
+      </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>50</v>
       </c>
@@ -5657,8 +5786,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K55">
+        <f t="shared" si="8"/>
+        <v>111.34638197484279</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="9"/>
+        <v>69.249896035986936</v>
+      </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>51</v>
       </c>
@@ -5694,8 +5831,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K56">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -5731,8 +5876,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K57">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>53</v>
       </c>
@@ -5768,8 +5921,16 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K58">
+        <f t="shared" si="8"/>
+        <v>92.918332839255498</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="9"/>
+        <v>69.867328586742232</v>
+      </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -5805,8 +5966,16 @@
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
+      <c r="K59">
+        <f t="shared" si="8"/>
+        <v>89.274476649480775</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="9"/>
+        <v>69.16466392753712</v>
+      </c>
     </row>
-    <row r="60" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="18" t="s">
         <v>55</v>
       </c>
@@ -5842,82 +6011,146 @@
         <f t="shared" si="7"/>
         <v>5.5</v>
       </c>
+      <c r="K60" s="17">
+        <f t="shared" si="8"/>
+        <v>82.454137516586599</v>
+      </c>
+      <c r="L60" s="18">
+        <f t="shared" si="9"/>
+        <v>70.230655737065248</v>
+      </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C61" s="23">
         <f>AVERAGE(C43:C60)</f>
         <v>25.666666666666668</v>
       </c>
       <c r="D61" s="23">
-        <f t="shared" ref="D61:J61" si="8">AVERAGE(D43:D60)</f>
+        <f t="shared" ref="D61:L61" si="10">AVERAGE(D43:D60)</f>
         <v>12.722222222222221</v>
       </c>
       <c r="E61" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.5555555555555556</v>
       </c>
       <c r="F61" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
       <c r="G61" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.583333333333333</v>
       </c>
       <c r="H61" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.6111111111111107</v>
       </c>
       <c r="I61" s="23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>5.583333333333333</v>
       </c>
-      <c r="J61" s="23">
-        <f t="shared" si="8"/>
+      <c r="J61" s="25">
+        <f t="shared" si="10"/>
         <v>5.6111111111111107</v>
       </c>
-      <c r="K61" s="24">
-        <f>C61*LOG(D61,2)</f>
-        <v>94.178155524135562</v>
-      </c>
-      <c r="L61" s="25">
-        <f>MAX(0,(171 - 5.2 * LN(K61) - 0.23 * (E61) - 16.2 *LN(H61))*100 / 171)</f>
-        <v>69.629423026369253</v>
+      <c r="K61" s="23">
+        <f t="shared" si="10"/>
+        <v>94.224216647515505</v>
+      </c>
+      <c r="L61" s="23">
+        <f t="shared" si="10"/>
+        <v>69.649659092367841</v>
+      </c>
+      <c r="M61" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C62" s="20" t="s">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C62" s="23">
+        <f>_xlfn.STDEV.P(C43:C60)</f>
+        <v>1.6749792701868149</v>
+      </c>
+      <c r="D62" s="23">
+        <f t="shared" ref="D62:L62" si="11">_xlfn.STDEV.P(D43:D60)</f>
+        <v>0.90095970779038093</v>
+      </c>
+      <c r="E62" s="23">
+        <f t="shared" si="11"/>
+        <v>0.15713484026367722</v>
+      </c>
+      <c r="F62" s="23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="23">
+        <f t="shared" si="11"/>
+        <v>0.30046260628866578</v>
+      </c>
+      <c r="H62" s="23">
+        <f t="shared" si="11"/>
+        <v>0.26643508462848436</v>
+      </c>
+      <c r="I62" s="23">
+        <f t="shared" si="11"/>
+        <v>0.30046260628866578</v>
+      </c>
+      <c r="J62" s="24">
+        <f t="shared" si="11"/>
+        <v>0.26643508462848436</v>
+      </c>
+      <c r="K62" s="26">
+        <f t="shared" si="11"/>
+        <v>8.4427118326841555</v>
+      </c>
+      <c r="L62" s="27">
+        <f t="shared" si="11"/>
+        <v>0.59526347124650547</v>
+      </c>
+      <c r="M62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C63" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="21" t="s">
+      <c r="D63" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" s="20" t="s">
+      <c r="E63" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G63" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="H63" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I62" s="20" t="s">
+      <c r="I63" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J62" s="22" t="s">
+      <c r="J63" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="K62" s="20" t="s">
+      <c r="K63" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L62" s="20" t="s">
+      <c r="L63" s="20" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K64" s="23"/>
+      <c r="L64" s="23"/>
+      <c r="M64" s="23"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K41:L41"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="javascript:(function() %7bwindow.open('/code?id=Licca_C:Original.c&amp;line=1%27,%20%27Licca_C:Original.c%27,%20%27resizable,scrollbars,status%27);%7d)()"/>
     <hyperlink ref="A4" r:id="rId2" display="javascript:(function() %7bwindow.open('/code?id=Licca_C:S1a.c&amp;line=1%27,%20%27Licca_C:S1a.c%27,%20%27resizable,scrollbars,status%27);%7d)()"/>

</xml_diff>